<commit_message>
notes added on paper
</commit_message>
<xml_diff>
--- a/model_lca/building_lci.xlsx
+++ b/model_lca/building_lci.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15690" windowHeight="5810" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Unique inventories" sheetId="1" r:id="rId1"/>
     <sheet name="inventories" sheetId="2" r:id="rId2"/>
+    <sheet name="KBOB" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -630,8 +631,43 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rhythima Shinde:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>for materials: kg/m2a is provided 
+for energy MJ/m2 is provided, so lifetime of 80 years is assumed</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="99">
   <si>
     <t>name</t>
   </si>
@@ -892,6 +928,42 @@
   </si>
   <si>
     <t>Expanded polystyrene (EPS)</t>
+  </si>
+  <si>
+    <t>building 1</t>
+  </si>
+  <si>
+    <t>building 6</t>
+  </si>
+  <si>
+    <t>building 2</t>
+  </si>
+  <si>
+    <t>building 8</t>
+  </si>
+  <si>
+    <t>building 9</t>
+  </si>
+  <si>
+    <t>building 7</t>
+  </si>
+  <si>
+    <t>building 3</t>
+  </si>
+  <si>
+    <t>building 4</t>
+  </si>
+  <si>
+    <t>building 5</t>
+  </si>
+  <si>
+    <t>building 10</t>
+  </si>
+  <si>
+    <t>building 11</t>
+  </si>
+  <si>
+    <t>building 12</t>
   </si>
 </sst>
 </file>
@@ -1157,6 +1229,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1166,11 +1243,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1521,8 +1593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMH95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1538,28 +1610,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="25" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="27"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="26" t="s">
         <v>85</v>
       </c>
       <c r="D2" s="17" t="s">
@@ -1585,7 +1657,7 @@
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="27" t="s">
         <v>75</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1617,7 +1689,7 @@
       <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="27" t="s">
         <v>76</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -1649,7 +1721,7 @@
       <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="27" t="s">
         <v>86</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1681,7 +1753,7 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="27" t="s">
         <v>77</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1713,7 +1785,7 @@
       <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="27" t="s">
         <v>79</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -1745,7 +1817,7 @@
       <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="27" t="s">
         <v>80</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1777,7 +1849,7 @@
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="27" t="s">
         <v>78</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1809,7 +1881,7 @@
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="30"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="19" t="s">
@@ -1835,7 +1907,7 @@
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="27" t="s">
         <v>81</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -1867,7 +1939,7 @@
       <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="27" t="s">
         <v>82</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -1899,7 +1971,7 @@
       <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="30"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="19" t="s">
@@ -1925,7 +1997,7 @@
       <c r="M13" s="3"/>
     </row>
     <row r="14" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="27" t="s">
         <v>83</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1957,7 +2029,7 @@
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="27" t="s">
         <v>84</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -1989,7 +2061,7 @@
       <c r="M15" s="3"/>
     </row>
     <row r="16" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="27" t="s">
         <v>78</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -2021,9 +2093,9 @@
       <c r="M16" s="3"/>
     </row>
     <row r="17" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="31"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
       <c r="D17" s="21" t="s">
         <v>34</v>
       </c>
@@ -2441,7 +2513,7 @@
   <dimension ref="A1:AMJ361"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8867,4 +8939,1641 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="41.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="7">
+        <v>2.4820000000000002</v>
+      </c>
+      <c r="C2">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A2,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.223</v>
+      </c>
+      <c r="D2">
+        <f>C2*B2</f>
+        <v>0.55348600000000003</v>
+      </c>
+      <c r="G2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2">
+        <v>11.973719999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="7">
+        <v>23.141999999999999</v>
+      </c>
+      <c r="C3">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A3,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">C3*B3</f>
+        <v>9.6502140000000001</v>
+      </c>
+      <c r="G3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3">
+        <v>6.5177649999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="7">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="C4">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A4,'Unique inventories'!D$3:D$17,0))</f>
+        <v>7.64</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.74107999999999996</v>
+      </c>
+      <c r="G4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4">
+        <v>2.2061949999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C5">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A5,'Unique inventories'!D$3:D$17,0))</f>
+        <v>14.5</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.24650000000000002</v>
+      </c>
+      <c r="G5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5">
+        <v>8.1118649999999981</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="7">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C6">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A6,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>2.5989999999999996E-2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6">
+        <v>6.1315839999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="7">
+        <v>2.7E-2</v>
+      </c>
+      <c r="C7">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A7,'Unique inventories'!D$3:D$17,0))</f>
+        <v>7.52</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.20304</v>
+      </c>
+      <c r="G7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7">
+        <v>19.782176999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="C8">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A8,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.17</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.55340999999999996</v>
+      </c>
+      <c r="G8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8">
+        <v>9.7804249999999975</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" t="e">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A9,'Unique inventories'!D$3:D$17,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D9" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E9">
+        <f>SUM(D2:D8)</f>
+        <v>11.973719999999998</v>
+      </c>
+      <c r="G9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9">
+        <v>8.1722239999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="7">
+        <v>20.48</v>
+      </c>
+      <c r="C10">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A10,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>8.5401600000000002</v>
+      </c>
+      <c r="G10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10">
+        <v>7.4503129999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="C11">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A11,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.10929600000000002</v>
+      </c>
+      <c r="G11" t="s">
+        <v>96</v>
+      </c>
+      <c r="H11">
+        <v>7.9029620000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1.2410000000000001</v>
+      </c>
+      <c r="C12">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A12,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.601885</v>
+      </c>
+      <c r="G12" t="s">
+        <v>97</v>
+      </c>
+      <c r="H12">
+        <v>9.0742699999999985</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="7">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="C13">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A13,'Unique inventories'!D$3:D$17,0))</f>
+        <v>7.64</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.25975999999999999</v>
+      </c>
+      <c r="G13" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13">
+        <v>13.316568</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="C14">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A14,'Unique inventories'!D$3:D$17,0))</f>
+        <v>14.5</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>2.581</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1.363</v>
+      </c>
+      <c r="C15">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A15,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1.5401899999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="7">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="C16">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A16,'Unique inventories'!D$3:D$17,0))</f>
+        <v>7.52</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0.57904</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="C17">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A17,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.17</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.95588999999999991</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" t="e">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A18,'Unique inventories'!D$3:D$17,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D18" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E18">
+        <f>SUM(D12:D17)</f>
+        <v>6.5177649999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="7">
+        <v>8.1959999999999997</v>
+      </c>
+      <c r="C19">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A19,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>3.4177319999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="7">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C20">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A20,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>4.0920000000000002E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1.327</v>
+      </c>
+      <c r="C21">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A21,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0.64359499999999992</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="7">
+        <v>0.154</v>
+      </c>
+      <c r="C22">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A22,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>3.9578000000000002E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="7">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="C23">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A23,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.17</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0.19070999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="7">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="C24">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A24,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>0.75257999999999992</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="C25">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A25,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.17</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>0.57563999999999993</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="7">
+        <v>1</v>
+      </c>
+      <c r="C26" t="e">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A26,'Unique inventories'!D$3:D$17,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D26" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E26">
+        <f>SUM(D20:D25)</f>
+        <v>2.2061949999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="7">
+        <v>3.9609999999999999</v>
+      </c>
+      <c r="C27">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A27,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.223</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>0.88330299999999995</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="7">
+        <v>15.026</v>
+      </c>
+      <c r="C28">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A28,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>6.2658419999999992</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="7">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C29">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A29,'Unique inventories'!D$3:D$17,0))</f>
+        <v>7.64</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>0.48896000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="7">
+        <v>6.3E-2</v>
+      </c>
+      <c r="C30">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A30,'Unique inventories'!D$3:D$17,0))</f>
+        <v>7.52</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>0.47375999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="7">
+        <v>1</v>
+      </c>
+      <c r="C31" t="e">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A31,'Unique inventories'!D$3:D$17,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D31" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E31">
+        <f>SUM(D27:D30)</f>
+        <v>8.1118649999999981</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="7">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="C32">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A32,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.223</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>0.15030200000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="7">
+        <v>12.898</v>
+      </c>
+      <c r="C33">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A33,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>5.3784659999999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="7">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C34">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A34,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>8.8320000000000013E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="7">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C35">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A35,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>2.7280000000000004E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="7">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="C36">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A36,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>0.22601000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="7">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="C37">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A37,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>7.1446000000000009E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="C38">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A38,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>0.29380000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="7">
+        <v>1</v>
+      </c>
+      <c r="C39" t="e">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A39,'Unique inventories'!D$3:D$17,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D39" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E39">
+        <f>SUM(D32:D38)</f>
+        <v>6.1315839999999993</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="12">
+        <v>42.655000000000001</v>
+      </c>
+      <c r="C40">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A40,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>17.787134999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="12">
+        <v>0.626</v>
+      </c>
+      <c r="C41">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A41,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>8.6388000000000006E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="12">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="C42">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A42,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>0.41192800000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="C43">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A43,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>0.36375000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="12">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="C44">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A44,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>0.109996</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="12">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="C45">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A45,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>0.57177999999999995</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="C46">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A46,'Unique inventories'!D$3:D$17,0))</f>
+        <v>7.52</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>0.45119999999999993</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="7">
+        <v>1</v>
+      </c>
+      <c r="C47" t="e">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A47,'Unique inventories'!D$3:D$17,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D47" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E47">
+        <f>SUM(D40:D46)</f>
+        <v>19.782176999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="12">
+        <v>0.995</v>
+      </c>
+      <c r="C48">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A48,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.223</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>0.221885</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="12">
+        <v>20.79</v>
+      </c>
+      <c r="C49">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A49,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>8.6694299999999984</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" s="12">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="C50">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A50,'Unique inventories'!D$3:D$17,0))</f>
+        <v>7.64</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>0.22156000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C51">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A51,'Unique inventories'!D$3:D$17,0))</f>
+        <v>14.5</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="12">
+        <v>2.7E-2</v>
+      </c>
+      <c r="C52">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A52,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>3.0509999999999995E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" s="12">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="C53">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A53,'Unique inventories'!D$3:D$17,0))</f>
+        <v>7.52</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>0.57904</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="7">
+        <v>1</v>
+      </c>
+      <c r="C54" t="e">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A54,'Unique inventories'!D$3:D$17,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D54" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E54">
+        <f>SUM(D48:D53)</f>
+        <v>9.7804249999999975</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" s="12">
+        <v>13.163</v>
+      </c>
+      <c r="C55">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A55,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>5.4889710000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" s="12">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="C56">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A56,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>9.9498000000000003E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57" s="13">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="C57">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A57,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>0.37005500000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="12">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="C58">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A58,'Unique inventories'!D$3:D$17,0))</f>
+        <v>7.64</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>0.65703999999999996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="12">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="C59">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A59,'Unique inventories'!D$3:D$17,0))</f>
+        <v>14.5</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>0.88449999999999995</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B60" s="12">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="C60">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A60,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>0.31413999999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B61" s="13">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="C61">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A61,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.17</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>0.35801999999999995</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" s="7">
+        <v>1</v>
+      </c>
+      <c r="C62" t="e">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A62,'Unique inventories'!D$3:D$17,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D62" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E62">
+        <f>SUM(D55:D61)</f>
+        <v>8.1722239999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B63" s="16">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="C63">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A63,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.223</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>0.21697900000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" s="12">
+        <v>10.847</v>
+      </c>
+      <c r="C64">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A64,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>4.523199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" s="13">
+        <v>1.643</v>
+      </c>
+      <c r="C65">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A65,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>0.79685499999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B66" s="12">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="C66">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A66,'Unique inventories'!D$3:D$17,0))</f>
+        <v>7.64</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>0.90915999999999997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" s="12">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="C67">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A67,'Unique inventories'!D$3:D$17,0))</f>
+        <v>14.5</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D94" si="1">C67*B67</f>
+        <v>0.63800000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B68" s="12">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="C68">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A68,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="1"/>
+        <v>0.36612</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B69" s="7">
+        <v>1</v>
+      </c>
+      <c r="C69" t="e">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A69,'Unique inventories'!D$3:D$17,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D69" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E69">
+        <f>SUM(D63:D68)</f>
+        <v>7.4503129999999995</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" s="12">
+        <v>14.353</v>
+      </c>
+      <c r="C70">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A70,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="1"/>
+        <v>5.985201</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B71" s="12">
+        <v>6.7850000000000001</v>
+      </c>
+      <c r="C71">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A71,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="1"/>
+        <v>0.93633000000000011</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B72" s="13">
+        <v>0.06</v>
+      </c>
+      <c r="C72">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A72,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="1"/>
+        <v>2.9099999999999997E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B73" s="12">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="C73">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A73,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="1"/>
+        <v>2.3901000000000002E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B74" s="12">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="C74">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A74,'Unique inventories'!D$3:D$17,0))</f>
+        <v>7.64</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="1"/>
+        <v>0.44312000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B75" s="12">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="C75">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A75,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="1"/>
+        <v>0.36498999999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B76" s="12">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C76">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A76,'Unique inventories'!D$3:D$17,0))</f>
+        <v>7.52</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="1"/>
+        <v>0.12032</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B77" s="7">
+        <v>1</v>
+      </c>
+      <c r="C77" t="e">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A77,'Unique inventories'!D$3:D$17,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D77" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E77">
+        <f>SUM(D70:D76)</f>
+        <v>7.9029620000000005</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B78" s="12">
+        <v>1.0269999999999999</v>
+      </c>
+      <c r="C78">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A78,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.223</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="1"/>
+        <v>0.22902099999999997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B79" s="12">
+        <v>15.727</v>
+      </c>
+      <c r="C79">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A79,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="1"/>
+        <v>6.5581589999999998</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B80" s="12">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C80">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A80,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="1"/>
+        <v>2.3870000000000002E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B81" s="12">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="C81">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A81,'Unique inventories'!D$3:D$17,0))</f>
+        <v>7.64</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="1"/>
+        <v>0.55771999999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B82" s="12">
+        <v>6.2E-2</v>
+      </c>
+      <c r="C82">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A82,'Unique inventories'!D$3:D$17,0))</f>
+        <v>14.5</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="1"/>
+        <v>0.89900000000000002</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B83" s="12">
+        <v>4.7E-2</v>
+      </c>
+      <c r="C83">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A83,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="1"/>
+        <v>5.3109999999999997E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B84" s="12">
+        <v>6.3E-2</v>
+      </c>
+      <c r="C84">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A84,'Unique inventories'!D$3:D$17,0))</f>
+        <v>7.52</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="1"/>
+        <v>0.47375999999999996</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B85" s="13">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="C85">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A85,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.17</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="1"/>
+        <v>0.27962999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B86" s="7">
+        <v>1</v>
+      </c>
+      <c r="C86" t="e">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A86,'Unique inventories'!D$3:D$17,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D86" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E86">
+        <f>SUM(D78:D85)</f>
+        <v>9.0742699999999985</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B87" s="12">
+        <v>24.609000000000002</v>
+      </c>
+      <c r="C87">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A87,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="1"/>
+        <v>10.261953</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B88" s="12">
+        <v>0.16</v>
+      </c>
+      <c r="C88">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A88,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="1"/>
+        <v>0.10912000000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B89" s="13">
+        <v>1.0549999999999999</v>
+      </c>
+      <c r="C89">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A89,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="1"/>
+        <v>0.51167499999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B90" s="12">
+        <v>0.09</v>
+      </c>
+      <c r="C90">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A90,'Unique inventories'!D$3:D$17,0))</f>
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="1"/>
+        <v>2.3130000000000001E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B91" s="12">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="C91">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A91,'Unique inventories'!D$3:D$17,0))</f>
+        <v>7.64</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="1"/>
+        <v>1.1001599999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B92" s="12">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="C92">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A92,'Unique inventories'!D$3:D$17,0))</f>
+        <v>14.5</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="1"/>
+        <v>0.71050000000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B93" s="12">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="C93">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A93,'Unique inventories'!D$3:D$17,0))</f>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="1"/>
+        <v>0.60002999999999995</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B94" s="7">
+        <v>1</v>
+      </c>
+      <c r="C94" t="e">
+        <f>INDEX('Unique inventories'!C$3:C$17,MATCH(KBOB!A94,'Unique inventories'!D$3:D$17,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D94" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E94">
+        <f>SUM(D87:D93)</f>
+        <v>13.316568</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>